<commit_message>
Geocoding - test cases v2
</commit_message>
<xml_diff>
--- a/Geocoding - test cases.xlsx
+++ b/Geocoding - test cases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Archi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Archi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="test cases" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="139">
   <si>
     <t>#</t>
   </si>
@@ -291,19 +291,151 @@
     <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxxxxxxx&amp;result_type=administrative_area_level_5&amp;key=YOUR_API_KEY</t>
   </si>
   <si>
-    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxxxx&amp;result_type=administrative_area_level_1&amp;key=YOUR_API_KEY</t>
-  </si>
-  <si>
-    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxxx,xxxx&amp;result_type=administrative_area_level_1&amp;key=YOUR_API_KEY</t>
-  </si>
-  <si>
-    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,-xxxx&amp;result_type=administrative_area_level_1&amp;key=YOUR_API_KEY</t>
-  </si>
-  <si>
-    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxx,xxxx&amp;result_type=administrative_area_level_1&amp;key=YOUR_API_KEY</t>
-  </si>
-  <si>
-    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,xxxx&amp;result_type=administrative_area_level_1&amp;key=YOUR_API_KEY</t>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=coloquial_area), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxxxx&amp;result_type=coloquial_area&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=locality), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,xxx&amp;result_type=locality&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=ward), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxxx,xxxx&amp;result_type=ward&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=sublocality), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,-xxxx&amp;result_type=sublocality&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=neighborhood), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxx,xxxx&amp;result_type=neighborhood&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=premise), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=subpremise), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxxx,xxxx&amp;result_type=premise&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,xxxx&amp;result_type=subpremise&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=postal_code), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxxx,xxxx&amp;result_type=postal_code&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=natural_feature), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,xxxx&amp;result_type=natural_feature&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=airport), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=park), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, result type=point_of_interest, verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,xxxx&amp;result_type=airport&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxxx,xxxx&amp;result_type=park&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,xxxx&amp;result_type=point_of_interest&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, location_type=ROOFTOP), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,xxxx&amp;location_type=ROOFTOP&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,xxxx&amp;location_type=RANGE_INTERPOLATED&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxxx,xxxx&amp;location_type=GEOMETRIC_CENTER&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>API URL: https://maps.googleapis.com/maps/api/geocode/json?latlng=xxxx,xxxx&amp;location_type=APROXIMATE&amp;key=YOUR_API_KEY</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, location_type=APROXIMATE), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, location_type=GEOMETRIC_CENTER), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude, latitude, location_type=RANGE_INTERPOLATED), verify street address and status (Status: OK)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=airport), verify status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=park), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, location_type=ROOFTOP), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=point_of_interest, verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, location_type=GEOMETRIC_CENTER), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude-invalid, latitude, location_type=RANGE_INTERPOLATED), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with valid parameters (longitude-invalid, latitude, location_type=APROXIMATE), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=administrative_area_level_5), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=coloquial_area), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=locality), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=ward), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=sublocality), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=neighborhood), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=premise), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-INVALID, latitude, result type=subpremise), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=postal_code), verify street address and status (Status: ZERO_RESULT)</t>
+  </si>
+  <si>
+    <t>Make an API call with invalid parameters (longitude-invalid, latitude, result type=natural_feature), verify street address and status (Status: ZERO_RESULT)</t>
   </si>
 </sst>
 </file>
@@ -736,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G193"/>
+  <dimension ref="A1:G348"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D6"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D349" sqref="D349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2891,7 +3023,7 @@
         <v>21</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
       <c r="E152" s="3" t="s">
         <v>10</v>
@@ -2913,7 +3045,7 @@
         <v>13</v>
       </c>
       <c r="G153" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.2">
@@ -2975,7 +3107,7 @@
         <v>21</v>
       </c>
       <c r="D158" s="6" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="E158" s="3" t="s">
         <v>10</v>
@@ -2997,7 +3129,7 @@
         <v>13</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.2">
@@ -3059,7 +3191,7 @@
         <v>21</v>
       </c>
       <c r="D164" s="6" t="s">
-        <v>65</v>
+        <v>94</v>
       </c>
       <c r="E164" s="3" t="s">
         <v>10</v>
@@ -3081,7 +3213,7 @@
         <v>13</v>
       </c>
       <c r="G165" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.2">
@@ -3143,7 +3275,7 @@
         <v>21</v>
       </c>
       <c r="D170" s="6" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="E170" s="3" t="s">
         <v>10</v>
@@ -3165,7 +3297,7 @@
         <v>13</v>
       </c>
       <c r="G171" s="3" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.2">
@@ -3227,7 +3359,7 @@
         <v>21</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>65</v>
+        <v>98</v>
       </c>
       <c r="E176" s="3" t="s">
         <v>10</v>
@@ -3249,7 +3381,7 @@
         <v>13</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.2">
@@ -3311,7 +3443,7 @@
         <v>21</v>
       </c>
       <c r="D182" s="6" t="s">
-        <v>65</v>
+        <v>100</v>
       </c>
       <c r="E182" s="3" t="s">
         <v>10</v>
@@ -3333,7 +3465,7 @@
         <v>13</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.2">
@@ -3395,7 +3527,7 @@
         <v>21</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>65</v>
+        <v>101</v>
       </c>
       <c r="E188" s="3" t="s">
         <v>10</v>
@@ -3417,7 +3549,7 @@
         <v>13</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.2">
@@ -3468,8 +3600,2223 @@
       <c r="F193" s="1"/>
       <c r="G193" s="2"/>
     </row>
+    <row r="194" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A194" s="6">
+        <v>33</v>
+      </c>
+      <c r="B194" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C194" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D194" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F194" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G194" s="3"/>
+    </row>
+    <row r="195" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A195" s="7"/>
+      <c r="B195" s="7"/>
+      <c r="C195" s="7"/>
+      <c r="D195" s="7"/>
+      <c r="E195" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F195" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G195" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="196" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A196" s="7"/>
+      <c r="B196" s="7"/>
+      <c r="C196" s="7"/>
+      <c r="D196" s="7"/>
+      <c r="E196" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F196" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G196" s="3"/>
+    </row>
+    <row r="197" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A197" s="7"/>
+      <c r="B197" s="7"/>
+      <c r="C197" s="7"/>
+      <c r="D197" s="7"/>
+      <c r="E197" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F197" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G197" s="3"/>
+    </row>
+    <row r="198" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A198" s="8"/>
+      <c r="B198" s="8"/>
+      <c r="C198" s="8"/>
+      <c r="D198" s="8"/>
+      <c r="E198" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F198" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G198" s="3"/>
+    </row>
+    <row r="199" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A199" s="5"/>
+      <c r="B199" s="5"/>
+      <c r="C199" s="5"/>
+      <c r="D199" s="5"/>
+      <c r="E199" s="1"/>
+      <c r="F199" s="1"/>
+      <c r="G199" s="2"/>
+    </row>
+    <row r="200" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A200" s="6">
+        <v>34</v>
+      </c>
+      <c r="B200" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C200" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D200" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="E200" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F200" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G200" s="3"/>
+    </row>
+    <row r="201" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A201" s="7"/>
+      <c r="B201" s="7"/>
+      <c r="C201" s="7"/>
+      <c r="D201" s="7"/>
+      <c r="E201" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F201" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G201" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="202" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A202" s="7"/>
+      <c r="B202" s="7"/>
+      <c r="C202" s="7"/>
+      <c r="D202" s="7"/>
+      <c r="E202" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F202" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G202" s="3"/>
+    </row>
+    <row r="203" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A203" s="7"/>
+      <c r="B203" s="7"/>
+      <c r="C203" s="7"/>
+      <c r="D203" s="7"/>
+      <c r="E203" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F203" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G203" s="3"/>
+    </row>
+    <row r="204" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A204" s="8"/>
+      <c r="B204" s="8"/>
+      <c r="C204" s="8"/>
+      <c r="D204" s="8"/>
+      <c r="E204" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F204" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G204" s="3"/>
+    </row>
+    <row r="205" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A205" s="2"/>
+      <c r="B205" s="2"/>
+      <c r="C205" s="2"/>
+      <c r="D205" s="2"/>
+      <c r="E205" s="1"/>
+      <c r="F205" s="1"/>
+      <c r="G205" s="2"/>
+    </row>
+    <row r="206" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A206" s="6">
+        <v>35</v>
+      </c>
+      <c r="B206" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C206" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D206" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="E206" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F206" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G206" s="3"/>
+    </row>
+    <row r="207" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A207" s="7"/>
+      <c r="B207" s="7"/>
+      <c r="C207" s="7"/>
+      <c r="D207" s="7"/>
+      <c r="E207" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F207" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G207" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="208" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A208" s="7"/>
+      <c r="B208" s="7"/>
+      <c r="C208" s="7"/>
+      <c r="D208" s="7"/>
+      <c r="E208" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F208" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G208" s="3"/>
+    </row>
+    <row r="209" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A209" s="7"/>
+      <c r="B209" s="7"/>
+      <c r="C209" s="7"/>
+      <c r="D209" s="7"/>
+      <c r="E209" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F209" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G209" s="3"/>
+    </row>
+    <row r="210" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A210" s="8"/>
+      <c r="B210" s="8"/>
+      <c r="C210" s="8"/>
+      <c r="D210" s="8"/>
+      <c r="E210" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F210" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G210" s="3"/>
+    </row>
+    <row r="211" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A211" s="2"/>
+      <c r="B211" s="2"/>
+      <c r="C211" s="2"/>
+      <c r="D211" s="2"/>
+      <c r="E211" s="1"/>
+      <c r="F211" s="1"/>
+      <c r="G211" s="2"/>
+    </row>
+    <row r="212" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A212" s="6">
+        <v>36</v>
+      </c>
+      <c r="B212" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C212" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D212" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="E212" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F212" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G212" s="3"/>
+    </row>
+    <row r="213" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A213" s="7"/>
+      <c r="B213" s="7"/>
+      <c r="C213" s="7"/>
+      <c r="D213" s="7"/>
+      <c r="E213" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F213" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G213" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="214" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A214" s="7"/>
+      <c r="B214" s="7"/>
+      <c r="C214" s="7"/>
+      <c r="D214" s="7"/>
+      <c r="E214" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F214" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G214" s="3"/>
+    </row>
+    <row r="215" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A215" s="7"/>
+      <c r="B215" s="7"/>
+      <c r="C215" s="7"/>
+      <c r="D215" s="7"/>
+      <c r="E215" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F215" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G215" s="3"/>
+    </row>
+    <row r="216" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A216" s="8"/>
+      <c r="B216" s="8"/>
+      <c r="C216" s="8"/>
+      <c r="D216" s="8"/>
+      <c r="E216" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F216" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G216" s="3"/>
+    </row>
+    <row r="217" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A217" s="5"/>
+      <c r="B217" s="5"/>
+      <c r="C217" s="5"/>
+      <c r="D217" s="5"/>
+      <c r="E217" s="1"/>
+      <c r="F217" s="1"/>
+      <c r="G217" s="2"/>
+    </row>
+    <row r="218" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A218" s="6">
+        <v>37</v>
+      </c>
+      <c r="B218" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C218" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D218" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="E218" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F218" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G218" s="3"/>
+    </row>
+    <row r="219" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A219" s="7"/>
+      <c r="B219" s="7"/>
+      <c r="C219" s="7"/>
+      <c r="D219" s="7"/>
+      <c r="E219" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F219" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G219" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="220" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A220" s="7"/>
+      <c r="B220" s="7"/>
+      <c r="C220" s="7"/>
+      <c r="D220" s="7"/>
+      <c r="E220" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F220" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G220" s="3"/>
+    </row>
+    <row r="221" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A221" s="7"/>
+      <c r="B221" s="7"/>
+      <c r="C221" s="7"/>
+      <c r="D221" s="7"/>
+      <c r="E221" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F221" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G221" s="3"/>
+    </row>
+    <row r="222" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A222" s="8"/>
+      <c r="B222" s="8"/>
+      <c r="C222" s="8"/>
+      <c r="D222" s="8"/>
+      <c r="E222" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F222" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G222" s="3"/>
+    </row>
+    <row r="223" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A223" s="2"/>
+      <c r="B223" s="2"/>
+      <c r="C223" s="2"/>
+      <c r="D223" s="2"/>
+      <c r="E223" s="1"/>
+      <c r="F223" s="1"/>
+      <c r="G223" s="2"/>
+    </row>
+    <row r="224" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A224" s="6">
+        <v>38</v>
+      </c>
+      <c r="B224" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C224" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D224" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="E224" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F224" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G224" s="3"/>
+    </row>
+    <row r="225" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A225" s="7"/>
+      <c r="B225" s="7"/>
+      <c r="C225" s="7"/>
+      <c r="D225" s="7"/>
+      <c r="E225" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F225" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G225" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="226" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A226" s="7"/>
+      <c r="B226" s="7"/>
+      <c r="C226" s="7"/>
+      <c r="D226" s="7"/>
+      <c r="E226" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F226" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G226" s="3"/>
+    </row>
+    <row r="227" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A227" s="7"/>
+      <c r="B227" s="7"/>
+      <c r="C227" s="7"/>
+      <c r="D227" s="7"/>
+      <c r="E227" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F227" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G227" s="3"/>
+    </row>
+    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A228" s="8"/>
+      <c r="B228" s="8"/>
+      <c r="C228" s="8"/>
+      <c r="D228" s="8"/>
+      <c r="E228" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F228" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G228" s="3"/>
+    </row>
+    <row r="229" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A229" s="2"/>
+      <c r="B229" s="2"/>
+      <c r="C229" s="2"/>
+      <c r="D229" s="2"/>
+      <c r="E229" s="1"/>
+      <c r="F229" s="1"/>
+      <c r="G229" s="2"/>
+    </row>
+    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A230" s="6">
+        <v>39</v>
+      </c>
+      <c r="B230" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C230" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D230" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E230" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F230" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G230" s="3"/>
+    </row>
+    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A231" s="7"/>
+      <c r="B231" s="7"/>
+      <c r="C231" s="7"/>
+      <c r="D231" s="7"/>
+      <c r="E231" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F231" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G231" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A232" s="7"/>
+      <c r="B232" s="7"/>
+      <c r="C232" s="7"/>
+      <c r="D232" s="7"/>
+      <c r="E232" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F232" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G232" s="3"/>
+    </row>
+    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A233" s="7"/>
+      <c r="B233" s="7"/>
+      <c r="C233" s="7"/>
+      <c r="D233" s="7"/>
+      <c r="E233" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F233" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G233" s="3"/>
+    </row>
+    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A234" s="8"/>
+      <c r="B234" s="8"/>
+      <c r="C234" s="8"/>
+      <c r="D234" s="8"/>
+      <c r="E234" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F234" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G234" s="3"/>
+    </row>
+    <row r="235" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A235" s="2"/>
+      <c r="B235" s="2"/>
+      <c r="C235" s="2"/>
+      <c r="D235" s="2"/>
+      <c r="E235" s="1"/>
+      <c r="F235" s="1"/>
+      <c r="G235" s="2"/>
+    </row>
+    <row r="236" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A236" s="6">
+        <v>40</v>
+      </c>
+      <c r="B236" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C236" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D236" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="E236" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F236" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G236" s="3"/>
+    </row>
+    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A237" s="7"/>
+      <c r="B237" s="7"/>
+      <c r="C237" s="7"/>
+      <c r="D237" s="7"/>
+      <c r="E237" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F237" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G237" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="238" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A238" s="7"/>
+      <c r="B238" s="7"/>
+      <c r="C238" s="7"/>
+      <c r="D238" s="7"/>
+      <c r="E238" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F238" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G238" s="3"/>
+    </row>
+    <row r="239" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A239" s="7"/>
+      <c r="B239" s="7"/>
+      <c r="C239" s="7"/>
+      <c r="D239" s="7"/>
+      <c r="E239" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F239" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G239" s="3"/>
+    </row>
+    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A240" s="8"/>
+      <c r="B240" s="8"/>
+      <c r="C240" s="8"/>
+      <c r="D240" s="8"/>
+      <c r="E240" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F240" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G240" s="3"/>
+    </row>
+    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A241" s="5"/>
+      <c r="B241" s="5"/>
+      <c r="C241" s="5"/>
+      <c r="D241" s="5"/>
+      <c r="E241" s="1"/>
+      <c r="F241" s="1"/>
+      <c r="G241" s="2"/>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A242" s="6">
+        <v>41</v>
+      </c>
+      <c r="B242" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C242" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D242" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E242" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F242" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G242" s="3"/>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A243" s="7"/>
+      <c r="B243" s="7"/>
+      <c r="C243" s="7"/>
+      <c r="D243" s="7"/>
+      <c r="E243" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F243" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G243" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A244" s="7"/>
+      <c r="B244" s="7"/>
+      <c r="C244" s="7"/>
+      <c r="D244" s="7"/>
+      <c r="E244" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F244" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G244" s="3"/>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A245" s="7"/>
+      <c r="B245" s="7"/>
+      <c r="C245" s="7"/>
+      <c r="D245" s="7"/>
+      <c r="E245" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F245" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G245" s="3"/>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A246" s="8"/>
+      <c r="B246" s="8"/>
+      <c r="C246" s="8"/>
+      <c r="D246" s="8"/>
+      <c r="E246" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F246" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G246" s="3"/>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A247" s="2"/>
+      <c r="B247" s="2"/>
+      <c r="C247" s="2"/>
+      <c r="D247" s="2"/>
+      <c r="E247" s="1"/>
+      <c r="F247" s="1"/>
+      <c r="G247" s="2"/>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A248" s="6">
+        <v>42</v>
+      </c>
+      <c r="B248" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C248" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D248" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="E248" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F248" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G248" s="3"/>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A249" s="7"/>
+      <c r="B249" s="7"/>
+      <c r="C249" s="7"/>
+      <c r="D249" s="7"/>
+      <c r="E249" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F249" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G249" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A250" s="7"/>
+      <c r="B250" s="7"/>
+      <c r="C250" s="7"/>
+      <c r="D250" s="7"/>
+      <c r="E250" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F250" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G250" s="3"/>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A251" s="7"/>
+      <c r="B251" s="7"/>
+      <c r="C251" s="7"/>
+      <c r="D251" s="7"/>
+      <c r="E251" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F251" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G251" s="3"/>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A252" s="8"/>
+      <c r="B252" s="8"/>
+      <c r="C252" s="8"/>
+      <c r="D252" s="8"/>
+      <c r="E252" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F252" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G252" s="3"/>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A253" s="2"/>
+      <c r="B253" s="2"/>
+      <c r="C253" s="2"/>
+      <c r="D253" s="2"/>
+      <c r="E253" s="1"/>
+      <c r="F253" s="1"/>
+      <c r="G253" s="2"/>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A254" s="6">
+        <v>43</v>
+      </c>
+      <c r="B254" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C254" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D254" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="E254" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F254" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G254" s="3"/>
+    </row>
+    <row r="255" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A255" s="7"/>
+      <c r="B255" s="7"/>
+      <c r="C255" s="7"/>
+      <c r="D255" s="7"/>
+      <c r="E255" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F255" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G255" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="256" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A256" s="7"/>
+      <c r="B256" s="7"/>
+      <c r="C256" s="7"/>
+      <c r="D256" s="7"/>
+      <c r="E256" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F256" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G256" s="3"/>
+    </row>
+    <row r="257" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A257" s="7"/>
+      <c r="B257" s="7"/>
+      <c r="C257" s="7"/>
+      <c r="D257" s="7"/>
+      <c r="E257" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F257" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G257" s="3"/>
+    </row>
+    <row r="258" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A258" s="8"/>
+      <c r="B258" s="8"/>
+      <c r="C258" s="8"/>
+      <c r="D258" s="8"/>
+      <c r="E258" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F258" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G258" s="3"/>
+    </row>
+    <row r="259" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A259" s="5"/>
+      <c r="B259" s="5"/>
+      <c r="C259" s="5"/>
+      <c r="D259" s="5"/>
+      <c r="E259" s="1"/>
+      <c r="F259" s="1"/>
+      <c r="G259" s="2"/>
+    </row>
+    <row r="260" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A260" s="6">
+        <v>44</v>
+      </c>
+      <c r="B260" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C260" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D260" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="E260" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F260" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G260" s="3"/>
+    </row>
+    <row r="261" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A261" s="7"/>
+      <c r="B261" s="7"/>
+      <c r="C261" s="7"/>
+      <c r="D261" s="7"/>
+      <c r="E261" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F261" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G261" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="262" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A262" s="7"/>
+      <c r="B262" s="7"/>
+      <c r="C262" s="7"/>
+      <c r="D262" s="7"/>
+      <c r="E262" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F262" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G262" s="3"/>
+    </row>
+    <row r="263" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A263" s="7"/>
+      <c r="B263" s="7"/>
+      <c r="C263" s="7"/>
+      <c r="D263" s="7"/>
+      <c r="E263" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F263" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G263" s="3"/>
+    </row>
+    <row r="264" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A264" s="8"/>
+      <c r="B264" s="8"/>
+      <c r="C264" s="8"/>
+      <c r="D264" s="8"/>
+      <c r="E264" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F264" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G264" s="3"/>
+    </row>
+    <row r="265" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A265" s="2"/>
+      <c r="B265" s="2"/>
+      <c r="C265" s="2"/>
+      <c r="D265" s="2"/>
+      <c r="E265" s="1"/>
+      <c r="F265" s="1"/>
+      <c r="G265" s="2"/>
+    </row>
+    <row r="266" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A266" s="6">
+        <v>45</v>
+      </c>
+      <c r="B266" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C266" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D266" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="E266" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F266" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G266" s="3"/>
+    </row>
+    <row r="267" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A267" s="7"/>
+      <c r="B267" s="7"/>
+      <c r="C267" s="7"/>
+      <c r="D267" s="7"/>
+      <c r="E267" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F267" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G267" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="268" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A268" s="7"/>
+      <c r="B268" s="7"/>
+      <c r="C268" s="7"/>
+      <c r="D268" s="7"/>
+      <c r="E268" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F268" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G268" s="3"/>
+    </row>
+    <row r="269" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A269" s="7"/>
+      <c r="B269" s="7"/>
+      <c r="C269" s="7"/>
+      <c r="D269" s="7"/>
+      <c r="E269" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F269" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G269" s="3"/>
+    </row>
+    <row r="270" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A270" s="8"/>
+      <c r="B270" s="8"/>
+      <c r="C270" s="8"/>
+      <c r="D270" s="8"/>
+      <c r="E270" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F270" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G270" s="3"/>
+    </row>
+    <row r="271" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A271" s="2"/>
+      <c r="B271" s="2"/>
+      <c r="C271" s="2"/>
+      <c r="D271" s="2"/>
+      <c r="E271" s="1"/>
+      <c r="F271" s="1"/>
+      <c r="G271" s="2"/>
+    </row>
+    <row r="272" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A272" s="6">
+        <v>46</v>
+      </c>
+      <c r="B272" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C272" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D272" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="E272" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F272" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G272" s="3"/>
+    </row>
+    <row r="273" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A273" s="7"/>
+      <c r="B273" s="7"/>
+      <c r="C273" s="7"/>
+      <c r="D273" s="7"/>
+      <c r="E273" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F273" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G273" s="3" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="274" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A274" s="7"/>
+      <c r="B274" s="7"/>
+      <c r="C274" s="7"/>
+      <c r="D274" s="7"/>
+      <c r="E274" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F274" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G274" s="3"/>
+    </row>
+    <row r="275" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A275" s="7"/>
+      <c r="B275" s="7"/>
+      <c r="C275" s="7"/>
+      <c r="D275" s="7"/>
+      <c r="E275" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F275" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G275" s="3"/>
+    </row>
+    <row r="276" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A276" s="8"/>
+      <c r="B276" s="8"/>
+      <c r="C276" s="8"/>
+      <c r="D276" s="8"/>
+      <c r="E276" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F276" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G276" s="3"/>
+    </row>
+    <row r="277" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A277" s="2"/>
+      <c r="B277" s="2"/>
+      <c r="C277" s="2"/>
+      <c r="D277" s="2"/>
+      <c r="E277" s="1"/>
+      <c r="F277" s="1"/>
+      <c r="G277" s="2"/>
+    </row>
+    <row r="278" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A278" s="6">
+        <v>47</v>
+      </c>
+      <c r="B278" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C278" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D278" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="E278" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F278" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G278" s="3"/>
+    </row>
+    <row r="279" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A279" s="7"/>
+      <c r="B279" s="7"/>
+      <c r="C279" s="7"/>
+      <c r="D279" s="7"/>
+      <c r="E279" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F279" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G279" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A280" s="7"/>
+      <c r="B280" s="7"/>
+      <c r="C280" s="7"/>
+      <c r="D280" s="7"/>
+      <c r="E280" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F280" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G280" s="3"/>
+    </row>
+    <row r="281" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A281" s="7"/>
+      <c r="B281" s="7"/>
+      <c r="C281" s="7"/>
+      <c r="D281" s="7"/>
+      <c r="E281" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F281" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G281" s="3"/>
+    </row>
+    <row r="282" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A282" s="8"/>
+      <c r="B282" s="8"/>
+      <c r="C282" s="8"/>
+      <c r="D282" s="8"/>
+      <c r="E282" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F282" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G282" s="3"/>
+    </row>
+    <row r="283" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A283" s="5"/>
+      <c r="B283" s="5"/>
+      <c r="C283" s="5"/>
+      <c r="D283" s="5"/>
+      <c r="E283" s="1"/>
+      <c r="F283" s="1"/>
+      <c r="G283" s="2"/>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A284" s="6">
+        <v>48</v>
+      </c>
+      <c r="B284" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C284" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D284" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="E284" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F284" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G284" s="3"/>
+    </row>
+    <row r="285" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A285" s="7"/>
+      <c r="B285" s="7"/>
+      <c r="C285" s="7"/>
+      <c r="D285" s="7"/>
+      <c r="E285" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F285" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G285" s="3" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="286" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A286" s="7"/>
+      <c r="B286" s="7"/>
+      <c r="C286" s="7"/>
+      <c r="D286" s="7"/>
+      <c r="E286" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F286" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G286" s="3"/>
+    </row>
+    <row r="287" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A287" s="7"/>
+      <c r="B287" s="7"/>
+      <c r="C287" s="7"/>
+      <c r="D287" s="7"/>
+      <c r="E287" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F287" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G287" s="3"/>
+    </row>
+    <row r="288" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A288" s="8"/>
+      <c r="B288" s="8"/>
+      <c r="C288" s="8"/>
+      <c r="D288" s="8"/>
+      <c r="E288" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F288" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G288" s="3"/>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A289" s="2"/>
+      <c r="B289" s="2"/>
+      <c r="C289" s="2"/>
+      <c r="D289" s="2"/>
+      <c r="E289" s="1"/>
+      <c r="F289" s="1"/>
+      <c r="G289" s="2"/>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A290" s="6">
+        <v>49</v>
+      </c>
+      <c r="B290" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C290" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D290" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E290" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F290" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G290" s="3"/>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A291" s="7"/>
+      <c r="B291" s="7"/>
+      <c r="C291" s="7"/>
+      <c r="D291" s="7"/>
+      <c r="E291" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F291" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G291" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A292" s="7"/>
+      <c r="B292" s="7"/>
+      <c r="C292" s="7"/>
+      <c r="D292" s="7"/>
+      <c r="E292" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F292" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G292" s="3"/>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A293" s="7"/>
+      <c r="B293" s="7"/>
+      <c r="C293" s="7"/>
+      <c r="D293" s="7"/>
+      <c r="E293" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F293" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G293" s="3"/>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A294" s="8"/>
+      <c r="B294" s="8"/>
+      <c r="C294" s="8"/>
+      <c r="D294" s="8"/>
+      <c r="E294" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F294" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G294" s="3"/>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A295" s="5"/>
+      <c r="B295" s="5"/>
+      <c r="C295" s="5"/>
+      <c r="D295" s="5"/>
+      <c r="E295" s="1"/>
+      <c r="F295" s="1"/>
+      <c r="G295" s="2"/>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A296" s="6">
+        <v>50</v>
+      </c>
+      <c r="B296" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C296" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D296" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="E296" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F296" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G296" s="3"/>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A297" s="7"/>
+      <c r="B297" s="7"/>
+      <c r="C297" s="7"/>
+      <c r="D297" s="7"/>
+      <c r="E297" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F297" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G297" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A298" s="7"/>
+      <c r="B298" s="7"/>
+      <c r="C298" s="7"/>
+      <c r="D298" s="7"/>
+      <c r="E298" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F298" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G298" s="3"/>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A299" s="7"/>
+      <c r="B299" s="7"/>
+      <c r="C299" s="7"/>
+      <c r="D299" s="7"/>
+      <c r="E299" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F299" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G299" s="3"/>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A300" s="8"/>
+      <c r="B300" s="8"/>
+      <c r="C300" s="8"/>
+      <c r="D300" s="8"/>
+      <c r="E300" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F300" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G300" s="3"/>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A301" s="5"/>
+      <c r="B301" s="5"/>
+      <c r="C301" s="5"/>
+      <c r="D301" s="5"/>
+      <c r="E301" s="1"/>
+      <c r="F301" s="1"/>
+      <c r="G301" s="2"/>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A302" s="6">
+        <v>51</v>
+      </c>
+      <c r="B302" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C302" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D302" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E302" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F302" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G302" s="3"/>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A303" s="7"/>
+      <c r="B303" s="7"/>
+      <c r="C303" s="7"/>
+      <c r="D303" s="7"/>
+      <c r="E303" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F303" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G303" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A304" s="7"/>
+      <c r="B304" s="7"/>
+      <c r="C304" s="7"/>
+      <c r="D304" s="7"/>
+      <c r="E304" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F304" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G304" s="3"/>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A305" s="7"/>
+      <c r="B305" s="7"/>
+      <c r="C305" s="7"/>
+      <c r="D305" s="7"/>
+      <c r="E305" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F305" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G305" s="3"/>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A306" s="8"/>
+      <c r="B306" s="8"/>
+      <c r="C306" s="8"/>
+      <c r="D306" s="8"/>
+      <c r="E306" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F306" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G306" s="3"/>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A307" s="5"/>
+      <c r="B307" s="5"/>
+      <c r="C307" s="5"/>
+      <c r="D307" s="5"/>
+      <c r="E307" s="1"/>
+      <c r="F307" s="1"/>
+      <c r="G307" s="2"/>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A308" s="6">
+        <v>52</v>
+      </c>
+      <c r="B308" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C308" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D308" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E308" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F308" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G308" s="3"/>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A309" s="7"/>
+      <c r="B309" s="7"/>
+      <c r="C309" s="7"/>
+      <c r="D309" s="7"/>
+      <c r="E309" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F309" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G309" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A310" s="7"/>
+      <c r="B310" s="7"/>
+      <c r="C310" s="7"/>
+      <c r="D310" s="7"/>
+      <c r="E310" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F310" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G310" s="3"/>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A311" s="7"/>
+      <c r="B311" s="7"/>
+      <c r="C311" s="7"/>
+      <c r="D311" s="7"/>
+      <c r="E311" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F311" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G311" s="3"/>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A312" s="8"/>
+      <c r="B312" s="8"/>
+      <c r="C312" s="8"/>
+      <c r="D312" s="8"/>
+      <c r="E312" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F312" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G312" s="3"/>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A313" s="5"/>
+      <c r="B313" s="5"/>
+      <c r="C313" s="5"/>
+      <c r="D313" s="5"/>
+      <c r="E313" s="1"/>
+      <c r="F313" s="1"/>
+      <c r="G313" s="2"/>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A314" s="6">
+        <v>53</v>
+      </c>
+      <c r="B314" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C314" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D314" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E314" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F314" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G314" s="3"/>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A315" s="7"/>
+      <c r="B315" s="7"/>
+      <c r="C315" s="7"/>
+      <c r="D315" s="7"/>
+      <c r="E315" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F315" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G315" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A316" s="7"/>
+      <c r="B316" s="7"/>
+      <c r="C316" s="7"/>
+      <c r="D316" s="7"/>
+      <c r="E316" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F316" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G316" s="3"/>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A317" s="7"/>
+      <c r="B317" s="7"/>
+      <c r="C317" s="7"/>
+      <c r="D317" s="7"/>
+      <c r="E317" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F317" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G317" s="3"/>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A318" s="8"/>
+      <c r="B318" s="8"/>
+      <c r="C318" s="8"/>
+      <c r="D318" s="8"/>
+      <c r="E318" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F318" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G318" s="3"/>
+    </row>
+    <row r="319" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A319" s="5"/>
+      <c r="B319" s="5"/>
+      <c r="C319" s="5"/>
+      <c r="D319" s="5"/>
+      <c r="E319" s="1"/>
+      <c r="F319" s="1"/>
+      <c r="G319" s="2"/>
+    </row>
+    <row r="320" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A320" s="6">
+        <v>54</v>
+      </c>
+      <c r="B320" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C320" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D320" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="E320" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F320" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G320" s="3"/>
+    </row>
+    <row r="321" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A321" s="7"/>
+      <c r="B321" s="7"/>
+      <c r="C321" s="7"/>
+      <c r="D321" s="7"/>
+      <c r="E321" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F321" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G321" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="322" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A322" s="7"/>
+      <c r="B322" s="7"/>
+      <c r="C322" s="7"/>
+      <c r="D322" s="7"/>
+      <c r="E322" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F322" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G322" s="3"/>
+    </row>
+    <row r="323" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A323" s="7"/>
+      <c r="B323" s="7"/>
+      <c r="C323" s="7"/>
+      <c r="D323" s="7"/>
+      <c r="E323" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F323" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G323" s="3"/>
+    </row>
+    <row r="324" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A324" s="8"/>
+      <c r="B324" s="8"/>
+      <c r="C324" s="8"/>
+      <c r="D324" s="8"/>
+      <c r="E324" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F324" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G324" s="3"/>
+    </row>
+    <row r="325" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A325" s="5"/>
+      <c r="B325" s="5"/>
+      <c r="C325" s="5"/>
+      <c r="D325" s="5"/>
+      <c r="E325" s="1"/>
+      <c r="F325" s="1"/>
+      <c r="G325" s="2"/>
+    </row>
+    <row r="326" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A326" s="6">
+        <v>55</v>
+      </c>
+      <c r="B326" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C326" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D326" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E326" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F326" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G326" s="3"/>
+    </row>
+    <row r="327" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A327" s="7"/>
+      <c r="B327" s="7"/>
+      <c r="C327" s="7"/>
+      <c r="D327" s="7"/>
+      <c r="E327" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F327" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G327" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="328" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A328" s="7"/>
+      <c r="B328" s="7"/>
+      <c r="C328" s="7"/>
+      <c r="D328" s="7"/>
+      <c r="E328" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F328" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G328" s="3"/>
+    </row>
+    <row r="329" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A329" s="7"/>
+      <c r="B329" s="7"/>
+      <c r="C329" s="7"/>
+      <c r="D329" s="7"/>
+      <c r="E329" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F329" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G329" s="3"/>
+    </row>
+    <row r="330" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A330" s="8"/>
+      <c r="B330" s="8"/>
+      <c r="C330" s="8"/>
+      <c r="D330" s="8"/>
+      <c r="E330" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F330" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G330" s="3"/>
+    </row>
+    <row r="331" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A331" s="5"/>
+      <c r="B331" s="5"/>
+      <c r="C331" s="5"/>
+      <c r="D331" s="5"/>
+      <c r="E331" s="1"/>
+      <c r="F331" s="1"/>
+      <c r="G331" s="2"/>
+    </row>
+    <row r="332" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A332" s="6">
+        <v>56</v>
+      </c>
+      <c r="B332" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C332" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D332" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="E332" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F332" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G332" s="3"/>
+    </row>
+    <row r="333" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A333" s="7"/>
+      <c r="B333" s="7"/>
+      <c r="C333" s="7"/>
+      <c r="D333" s="7"/>
+      <c r="E333" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F333" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G333" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="334" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A334" s="7"/>
+      <c r="B334" s="7"/>
+      <c r="C334" s="7"/>
+      <c r="D334" s="7"/>
+      <c r="E334" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F334" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G334" s="3"/>
+    </row>
+    <row r="335" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A335" s="7"/>
+      <c r="B335" s="7"/>
+      <c r="C335" s="7"/>
+      <c r="D335" s="7"/>
+      <c r="E335" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F335" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G335" s="3"/>
+    </row>
+    <row r="336" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A336" s="8"/>
+      <c r="B336" s="8"/>
+      <c r="C336" s="8"/>
+      <c r="D336" s="8"/>
+      <c r="E336" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F336" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G336" s="3"/>
+    </row>
+    <row r="337" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A337" s="2"/>
+      <c r="B337" s="2"/>
+      <c r="C337" s="2"/>
+      <c r="D337" s="2"/>
+      <c r="E337" s="1"/>
+      <c r="F337" s="1"/>
+      <c r="G337" s="2"/>
+    </row>
+    <row r="338" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A338" s="6">
+        <v>57</v>
+      </c>
+      <c r="B338" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C338" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D338" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E338" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F338" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G338" s="3"/>
+    </row>
+    <row r="339" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A339" s="7"/>
+      <c r="B339" s="7"/>
+      <c r="C339" s="7"/>
+      <c r="D339" s="7"/>
+      <c r="E339" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F339" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G339" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="340" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A340" s="7"/>
+      <c r="B340" s="7"/>
+      <c r="C340" s="7"/>
+      <c r="D340" s="7"/>
+      <c r="E340" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F340" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G340" s="3"/>
+    </row>
+    <row r="341" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A341" s="7"/>
+      <c r="B341" s="7"/>
+      <c r="C341" s="7"/>
+      <c r="D341" s="7"/>
+      <c r="E341" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F341" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G341" s="3"/>
+    </row>
+    <row r="342" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A342" s="8"/>
+      <c r="B342" s="8"/>
+      <c r="C342" s="8"/>
+      <c r="D342" s="8"/>
+      <c r="E342" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F342" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G342" s="3"/>
+    </row>
+    <row r="343" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A343" s="5"/>
+      <c r="B343" s="5"/>
+      <c r="C343" s="5"/>
+      <c r="D343" s="5"/>
+      <c r="E343" s="1"/>
+      <c r="F343" s="1"/>
+      <c r="G343" s="2"/>
+    </row>
+    <row r="344" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A344" s="6">
+        <v>58</v>
+      </c>
+      <c r="B344" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C344" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D344" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="E344" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F344" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G344" s="3"/>
+    </row>
+    <row r="345" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A345" s="7"/>
+      <c r="B345" s="7"/>
+      <c r="C345" s="7"/>
+      <c r="D345" s="7"/>
+      <c r="E345" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F345" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G345" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="346" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A346" s="7"/>
+      <c r="B346" s="7"/>
+      <c r="C346" s="7"/>
+      <c r="D346" s="7"/>
+      <c r="E346" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F346" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G346" s="3"/>
+    </row>
+    <row r="347" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A347" s="7"/>
+      <c r="B347" s="7"/>
+      <c r="C347" s="7"/>
+      <c r="D347" s="7"/>
+      <c r="E347" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F347" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G347" s="3"/>
+    </row>
+    <row r="348" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A348" s="8"/>
+      <c r="B348" s="8"/>
+      <c r="C348" s="8"/>
+      <c r="D348" s="8"/>
+      <c r="E348" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F348" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G348" s="3"/>
+    </row>
   </sheetData>
-  <mergeCells count="128">
+  <mergeCells count="232">
+    <mergeCell ref="A344:A348"/>
+    <mergeCell ref="B344:B348"/>
+    <mergeCell ref="C344:C348"/>
+    <mergeCell ref="D344:D348"/>
+    <mergeCell ref="A326:A330"/>
+    <mergeCell ref="B326:B330"/>
+    <mergeCell ref="C326:C330"/>
+    <mergeCell ref="D326:D330"/>
+    <mergeCell ref="A332:A336"/>
+    <mergeCell ref="B332:B336"/>
+    <mergeCell ref="C332:C336"/>
+    <mergeCell ref="D332:D336"/>
+    <mergeCell ref="A338:A342"/>
+    <mergeCell ref="B338:B342"/>
+    <mergeCell ref="C338:C342"/>
+    <mergeCell ref="D338:D342"/>
+    <mergeCell ref="A308:A312"/>
+    <mergeCell ref="B308:B312"/>
+    <mergeCell ref="C308:C312"/>
+    <mergeCell ref="D308:D312"/>
+    <mergeCell ref="A314:A318"/>
+    <mergeCell ref="B314:B318"/>
+    <mergeCell ref="C314:C318"/>
+    <mergeCell ref="D314:D318"/>
+    <mergeCell ref="A320:A324"/>
+    <mergeCell ref="B320:B324"/>
+    <mergeCell ref="C320:C324"/>
+    <mergeCell ref="D320:D324"/>
+    <mergeCell ref="A290:A294"/>
+    <mergeCell ref="B290:B294"/>
+    <mergeCell ref="C290:C294"/>
+    <mergeCell ref="D290:D294"/>
+    <mergeCell ref="A296:A300"/>
+    <mergeCell ref="B296:B300"/>
+    <mergeCell ref="C296:C300"/>
+    <mergeCell ref="D296:D300"/>
+    <mergeCell ref="A302:A306"/>
+    <mergeCell ref="B302:B306"/>
+    <mergeCell ref="C302:C306"/>
+    <mergeCell ref="D302:D306"/>
     <mergeCell ref="A2:A6"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="C2:C6"/>
@@ -3550,10 +5897,6 @@
     <mergeCell ref="C98:C102"/>
     <mergeCell ref="C92:C96"/>
     <mergeCell ref="C86:C90"/>
-    <mergeCell ref="C80:C84"/>
-    <mergeCell ref="C74:C78"/>
-    <mergeCell ref="B116:B120"/>
-    <mergeCell ref="B110:B114"/>
     <mergeCell ref="B104:B108"/>
     <mergeCell ref="B98:B102"/>
     <mergeCell ref="B92:B96"/>
@@ -3584,6 +5927,10 @@
     <mergeCell ref="B74:B78"/>
     <mergeCell ref="C128:C132"/>
     <mergeCell ref="C122:C126"/>
+    <mergeCell ref="C80:C84"/>
+    <mergeCell ref="C74:C78"/>
+    <mergeCell ref="B116:B120"/>
+    <mergeCell ref="B110:B114"/>
     <mergeCell ref="D164:D168"/>
     <mergeCell ref="D158:D162"/>
     <mergeCell ref="D152:D156"/>
@@ -3598,6 +5945,70 @@
     <mergeCell ref="C146:C150"/>
     <mergeCell ref="C140:C144"/>
     <mergeCell ref="C134:C138"/>
+    <mergeCell ref="A194:A198"/>
+    <mergeCell ref="B194:B198"/>
+    <mergeCell ref="C194:C198"/>
+    <mergeCell ref="D194:D198"/>
+    <mergeCell ref="A200:A204"/>
+    <mergeCell ref="B200:B204"/>
+    <mergeCell ref="C200:C204"/>
+    <mergeCell ref="D200:D204"/>
+    <mergeCell ref="A206:A210"/>
+    <mergeCell ref="B206:B210"/>
+    <mergeCell ref="C206:C210"/>
+    <mergeCell ref="D206:D210"/>
+    <mergeCell ref="A212:A216"/>
+    <mergeCell ref="B212:B216"/>
+    <mergeCell ref="C212:C216"/>
+    <mergeCell ref="D212:D216"/>
+    <mergeCell ref="A218:A222"/>
+    <mergeCell ref="B218:B222"/>
+    <mergeCell ref="C218:C222"/>
+    <mergeCell ref="D218:D222"/>
+    <mergeCell ref="A224:A228"/>
+    <mergeCell ref="B224:B228"/>
+    <mergeCell ref="C224:C228"/>
+    <mergeCell ref="D224:D228"/>
+    <mergeCell ref="A230:A234"/>
+    <mergeCell ref="B230:B234"/>
+    <mergeCell ref="C230:C234"/>
+    <mergeCell ref="D230:D234"/>
+    <mergeCell ref="A236:A240"/>
+    <mergeCell ref="B236:B240"/>
+    <mergeCell ref="C236:C240"/>
+    <mergeCell ref="D236:D240"/>
+    <mergeCell ref="A242:A246"/>
+    <mergeCell ref="B242:B246"/>
+    <mergeCell ref="C242:C246"/>
+    <mergeCell ref="D242:D246"/>
+    <mergeCell ref="A248:A252"/>
+    <mergeCell ref="B248:B252"/>
+    <mergeCell ref="C248:C252"/>
+    <mergeCell ref="D248:D252"/>
+    <mergeCell ref="A254:A258"/>
+    <mergeCell ref="B254:B258"/>
+    <mergeCell ref="C254:C258"/>
+    <mergeCell ref="D254:D258"/>
+    <mergeCell ref="A260:A264"/>
+    <mergeCell ref="B260:B264"/>
+    <mergeCell ref="C260:C264"/>
+    <mergeCell ref="D260:D264"/>
+    <mergeCell ref="A284:A288"/>
+    <mergeCell ref="B284:B288"/>
+    <mergeCell ref="C284:C288"/>
+    <mergeCell ref="D284:D288"/>
+    <mergeCell ref="A266:A270"/>
+    <mergeCell ref="B266:B270"/>
+    <mergeCell ref="C266:C270"/>
+    <mergeCell ref="D266:D270"/>
+    <mergeCell ref="A272:A276"/>
+    <mergeCell ref="B272:B276"/>
+    <mergeCell ref="C272:C276"/>
+    <mergeCell ref="D272:D276"/>
+    <mergeCell ref="A278:A282"/>
+    <mergeCell ref="B278:B282"/>
+    <mergeCell ref="C278:C282"/>
+    <mergeCell ref="D278:D282"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>